<commit_message>
everything works except for the next questions in the feedback page
</commit_message>
<xml_diff>
--- a/data/Easy_level_generated_dataset.xlsx
+++ b/data/Easy_level_generated_dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,46 +453,46 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Describe a time when you had to explain complex data to someone without a technical background.</t>
+          <t>What is the process of data analysis?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>When explaining complex data to someone without a technical background, it is important to simplify the concepts and use non-technical language. Begin by providing an overview of the data and its purpose. Break down complex terms and concepts into more understandable terms. Utilize visual aids, such as charts or graphs, to help illustrate the data. Additionally, it can be helpful to relate the data to real-world examples or scenarios that the person can relate to. For example, if discussing customer demographics, relate it to their own experiences as a consumer. Throughout the explanation, actively listen to any questions or concerns and be open to revisiting or clarifying information as needed.</t>
+          <t>Data analysis is a systematic process that involves inspecting, cleaning, transforming, and modeling data to extract useful information and support decision-making. The process begins with data collection, followed by data cleaning to eliminate errors or inconsistencies. Data transformation is done to convert data into a suitable format for analysis. Then, various analytical techniques, such as statistical analysis or data mining, are applied to explore patterns, relationships, or trends in the data. Finally, the results are interpreted and presented in a meaningful way to inform decision-making.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Behavioral</t>
+          <t>Technical</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Tell us about a project where you used data to solve a problem.</t>
+          <t>Can you describe the concept of data visualization?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>In a project where I used data to solve a problem, I was working for a retail company that wanted to optimize their inventory management. To solve this problem, I analyzed historical sales data to identify trends and patterns. I used statistical analysis techniques to forecast demand for different products and determine appropriate inventory levels. I also looked at customer purchase history to identify cross-selling opportunities. Based on my analysis, I recommended adjustments to the ordering and stocking processes. These recommendations resulted in improved inventory turnover, reduced stockouts, and increased sales. The project showcased my ability to collect and analyze data, derive actionable insights, and provide data-driven solutions to business problems.</t>
+          <t>Data visualization is the presentation of data in a graphical or visual format that facilitates understanding and interpretation. It involves the use of charts, graphs, maps, or other visual elements to represent data patterns, relationships, or trends. The primary purpose of data visualization is to make complex data more accessible, allowing users to identify patterns or outliers quickly and make informed decisions. By presenting data visually, it becomes easier to communicate insights, compare values, and understand the significance of the data. Effective data visualization enhances data analysis by providing a clear and concise representation of information.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Behavioral</t>
+          <t>Technical</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Describe a situation where you had to collect data from multiple sources. How did you ensure its accuracy?</t>
+          <t>Describe a time when you had to work under tight deadlines for a data analysis project.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>In a situation where I had to collect data from multiple sources, I was tasked with gathering customer feedback from surveys, social media, and customer service records. To ensure the accuracy of the data, I implemented several measures. First, I established clear criteria for data collection, ensuring consistent and relevant information across all sources. I also cross-checked the data from different sources to identify any inconsistencies or outliers. Additionally, I collaborated with the teams responsible for each data source to verify the accuracy of the data and address any discrepancies. By implementing strict data collection protocols and validation processes, I was able to ensure the accuracy and reliability of the data for analysis.</t>
+          <t>When answering this question, it is important to highlight your ability to work efficiently and effectively under pressure. Discuss a specific situation where you had to complete a data analysis project within a tight timeframe. Start by explaining the deadline and the importance of the project. Then, outline the steps you took to manage your time and prioritize tasks. Mention any strategies or techniques you used to streamline the data analysis process without compromising accuracy. Finally, share the outcome of the project and how you successfully met the deadline.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -504,29 +504,29 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>How do you prioritize tasks when working with multiple data sets?</t>
+          <t>Explain the concept of data normalization.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>When working with multiple data sets, I prioritize tasks based on their deadline, importance, and impact on the overall project. I start by evaluating the urgency of each task and identifying any dependencies or milestones. I then assess the importance of each task in achieving the project's objectives. I prioritize tasks that have a higher impact on the project's success or require immediate attention. To manage my priorities effectively, I utilize project management tools like Kanban boards or task trackers. These tools help me visualize the tasks, set deadlines, and allocate time accordingly. Regular communication with stakeholders and team members also helps me stay aligned and adjust task priorities as needed.</t>
+          <t>Data normalization is the process of organizing and structuring data to reduce redundancy and anomalies. It involves eliminating data duplication and ensuring data consistency by adhering to specific rules or normalization forms. The purpose of data normalization is to minimize data integrity issues, enhance data storage efficiency, and streamline data analysis. By normalizing data, you can eliminate data inconsistencies and improve the accuracy and reliability of analysis results. Common normalization techniques include splitting data into tables, creating relationships between tables, and applying normalization rules such as the first normal form (1NF), second normal form (2NF), and third normal form (3NF).</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Behavioral</t>
+          <t>Technical</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Can you give an example of how you have used data visualization to present findings?</t>
+          <t>Describe a situation where you had to present complex data findings to a non-technical audience.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Certainly! In a recent project, I was analyzing customer satisfaction data for a hospitality company. After conducting in-depth analysis, I needed to communicate my findings to the executive team, including non-technical stakeholders. To present the findings effectively, I used data visualization techniques. I created a series of interactive dashboards using Tableau that showcased key insights, trends, and customer sentiment. The visualizations included bar charts, line graphs, and geographical heatmaps. By using interactive elements, such as filters and drill-down functionalities, I allowed stakeholders to explore the data in a more engaging and customized manner. This approach made it easier for the team to grasp the insights quickly and facilitated data-driven decision-making.</t>
+          <t>When answering this question, focus on your ability to communicate complex information effectively. Start by explaining the context and the audience's level of technical knowledge. Outline the key insights or findings from your data analysis and consider how to simplify and present the information in a clear and concise manner. Use visual aids, such as charts or graphs, to support your explanation and make the data more accessible. Additionally, emphasize your communication skills, including the use of plain language, storytelling techniques, or analogies to help the audience understand the data. Finally, mention any feedback or questions received from the audience and how you addressed them.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -538,85 +538,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Can you share an experience where teamwork played a crucial role in a data analysis project?</t>
+          <t>What is the role of exploratory data analysis in the data analysis process?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Certainly! In a data analysis project I worked on, we were tasked with analyzing sales data and identifying key drivers of customer satisfaction. This involved gathering data from various sources, cleaning and transforming it, and conducting in-depth statistical analyses. Teamwork played a crucial role as we had to divide the workload, ensuring each team member had the necessary resources and support. We held regular meetings to discuss our progress, share insights, and align our analysis approaches. Collaboration was especially vital when it came to interpreting the results and drawing meaningful conclusions. By leveraging each team member's expertise and perspectives, we were able to deliver a comprehensive analysis that provided valuable insights and recommendations for the business.</t>
+          <t>Exploratory data analysis (EDA) is a critical step in the data analysis process. Its primary role is to gain insights and understand the data before applying more complex analysis techniques. During EDA, you explore the data to identify patterns, trends, or outliers. This involves the use of summary statistics, visualizations, and basic analytical techniques. EDA helps in understanding data quality, detecting data errors or missing values, and uncovering relationships or associations between variables. By gaining a deeper understanding of the data through EDA, you can make informed decisions about which analysis methods are appropriate and how to interpret the results accurately.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Behavioral</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Describe how you manage stress or tight deadlines in your data analysis work.</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>In my data analysis work, I manage stress and tight deadlines by employing several strategies. Firstly, I prioritize tasks and create a detailed work plan with specific deadlines. This allows me to allocate time effectively and ensures that critical tasks are completed on time. I also break down complex projects into smaller, manageable tasks, which helps in reducing overwhelm. Additionally, I practice time management techniques such as the Pomodoro Technique, where I work in focused sprints with short breaks in between. This helps me maintain productivity and avoid burnout. Moreover, I maintain open communication with stakeholders and team members, providing regular updates on progress and managing expectations. When facing tight deadlines, I remain calm and focused, seeking support or assistance when needed. By adopting these strategies, I can effectively manage stress and meet deadlines while maintaining the quality of my work.</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Behavioral</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Have you ever had to present your data findings to a non-technical audience? How did you approach it?</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Yes, I have frequently presented data findings to non-technical audiences. To effectively communicate complex data to individuals without a technical background, I follow several approaches. Firstly, I focus on identifying the key insights and messages that the audience needs to understand. I emphasize the practical implications of the data findings and connect them to the broader organizational goals or challenges. I avoid jargon or technical terms and use layman's language to explain concepts. Additionally, I utilize visual aids such as charts, graphs, and infographics to present the data in a clear and visually appealing manner. I also encourage audience participation by asking questions, allowing them to relate the data to their own experiences. Throughout the presentation, I remain attentive to audience engagement and adjust my approach accordingly to ensure comprehension and relevance.</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Behavioral</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Tell us about a time when you had to quickly adapt to a change in a data analysis project.</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>In a data analysis project, we were initially working with a specific dataset and had developed a detailed analysis plan. However, midway through the project, the client provided additional data that significantly expanded the scope and complexity of the analysis. To quickly adapt to this change, we assessed the new data for its relevance and impact on the project objectives. We revised our analysis plan to incorporate the new data and ensure a comprehensive and accurate analysis. This involved reevaluating our statistical models, adjusting our data cleansing processes, and expanding our visualization capabilities. We communicated the changes to the client, ensuring transparency and managing expectations. By proactively adapting to the change, we were able to deliver an enhanced analysis that provided deeper insights and addressed the client's evolving needs.</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Behavioral</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Describe a time when you had to learn something new at work. How did you approach this learning challenge?</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Learning new skills or technologies is a regular part of my work as a data analyst. When faced with a learning challenge, I approach it methodically and proactively. Firstly, I research and gather relevant resources, such as online tutorials, documentation, or training materials. I then create a learning plan, breaking down the new skill into smaller manageable components. This allows me to approach the learning process in a structured manner. During the learning process, I actively practice and apply the new knowledge through hands-on projects or simulations. I also seek guidance and support from colleagues or mentors, leveraging their expertise and experience. Once I have acquired the new skill, I reflect on the learning journey and identify areas for improvement or further exploration. By adopting this approach, I can effectively learn and integrate new skills into my data analysis work.</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Behavioral</t>
+          <t>Technical</t>
         </is>
       </c>
     </row>

</xml_diff>